<commit_message>
adding more scenarios and excel reader changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -50,7 +50,10 @@
     <t>Failure</t>
   </si>
   <si>
-    <t>RowIndex</t>
+    <t>Login_Invalid_Username</t>
+  </si>
+  <si>
+    <t>Login_Invalid_Password</t>
   </si>
   <si>
     <t>PythonCode</t>
@@ -59,7 +62,13 @@
     <t>ExpectedOutput</t>
   </si>
   <si>
+    <t>PythonCode_Valid</t>
+  </si>
+  <si>
     <t>print("Success")</t>
+  </si>
+  <si>
+    <t>PythonCode_Invalid</t>
   </si>
   <si>
     <t>print Failure</t>
@@ -374,6 +383,34 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -396,32 +433,32 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>0.0</v>
+      <c r="A2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>1.0</v>
+      <c r="A3" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>

</xml_diff>